<commit_message>
Corrected: designators,schematic documentation,text on pcb
</commit_message>
<xml_diff>
--- a/hardware/Default Configuration/Outputs/BOM/BOM_PartType-BatGPSTracker(WithoutRFMatching).xlsx
+++ b/hardware/Default Configuration/Outputs/BOM/BOM_PartType-BatGPSTracker(WithoutRFMatching).xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomfr\Documents\GitHub\gps_for_bats\hardware\Default Configuration\Outputs\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9108"/>
   </bookViews>
@@ -131,15 +136,6 @@
     <t>C3</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>C24</t>
-  </si>
-  <si>
     <t>IC4</t>
   </si>
   <si>
@@ -288,6 +284,15 @@
   </si>
   <si>
     <t>Bill of Materials</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
   </si>
 </sst>
 </file>
@@ -1344,8 +1349,8 @@
   </sheetPr>
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1484,11 +1489,11 @@
       <c r="E8" s="21"/>
       <c r="F8" s="24">
         <f ca="1">TODAY()</f>
-        <v>43528</v>
+        <v>43594</v>
       </c>
       <c r="G8" s="25">
         <f ca="1">NOW()</f>
-        <v>43528.469213310185</v>
+        <v>43594.53908923611</v>
       </c>
       <c r="H8" s="36"/>
       <c r="I8" s="23"/>
@@ -1509,13 +1514,13 @@
         <v>35</v>
       </c>
       <c r="F9" s="65" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G9" s="65" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H9" s="65" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I9" s="40" t="s">
         <v>24</v>
@@ -1527,7 +1532,7 @@
     <row r="10" spans="1:11" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
       <c r="B10" s="42">
-        <f>ROW(B10) - ROW($B$9)</f>
+        <f t="shared" ref="B10:B22" si="0">ROW(B10) - ROW($B$9)</f>
         <v>1</v>
       </c>
       <c r="C10" s="43"/>
@@ -1538,13 +1543,13 @@
         <v>36</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G10" s="66" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H10" s="66" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I10" s="44"/>
       <c r="J10" s="45"/>
@@ -1552,7 +1557,7 @@
     <row r="11" spans="1:11" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="46">
-        <f>ROW(B11) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C11" s="47"/>
@@ -1563,13 +1568,13 @@
         <v>37</v>
       </c>
       <c r="F11" s="67" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G11" s="67" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I11" s="47"/>
       <c r="J11" s="48"/>
@@ -1577,7 +1582,7 @@
     <row r="12" spans="1:11" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="37"/>
       <c r="B12" s="42">
-        <f>ROW(B12) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C12" s="43"/>
@@ -1585,16 +1590,16 @@
         <v>1</v>
       </c>
       <c r="E12" s="66" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G12" s="66" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H12" s="66" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I12" s="44"/>
       <c r="J12" s="45"/>
@@ -1602,7 +1607,7 @@
     <row r="13" spans="1:11" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="46">
-        <f>ROW(B13) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C13" s="47"/>
@@ -1610,16 +1615,16 @@
         <v>1</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="F13" s="67" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G13" s="67" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H13" s="67" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I13" s="47"/>
       <c r="J13" s="48"/>
@@ -1627,7 +1632,7 @@
     <row r="14" spans="1:11" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="42">
-        <f>ROW(B14) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C14" s="43"/>
@@ -1635,16 +1640,16 @@
         <v>1</v>
       </c>
       <c r="E14" s="66" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="F14" s="66" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G14" s="66" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H14" s="66" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I14" s="44"/>
       <c r="J14" s="45"/>
@@ -1652,7 +1657,7 @@
     <row r="15" spans="1:11" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37"/>
       <c r="B15" s="46">
-        <f>ROW(B15) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C15" s="47"/>
@@ -1660,16 +1665,16 @@
         <v>1</v>
       </c>
       <c r="E15" s="67" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F15" s="67" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G15" s="67" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H15" s="67" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I15" s="47"/>
       <c r="J15" s="48"/>
@@ -1677,7 +1682,7 @@
     <row r="16" spans="1:11" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37"/>
       <c r="B16" s="42">
-        <f>ROW(B16) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C16" s="43"/>
@@ -1685,16 +1690,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="66" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G16" s="66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H16" s="66" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I16" s="44"/>
       <c r="J16" s="45"/>
@@ -1702,7 +1707,7 @@
     <row r="17" spans="1:10" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="46">
-        <f>ROW(B17) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C17" s="47"/>
@@ -1710,16 +1715,16 @@
         <v>3</v>
       </c>
       <c r="E17" s="67" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F17" s="67" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G17" s="67" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H17" s="67" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I17" s="47"/>
       <c r="J17" s="48"/>
@@ -1727,7 +1732,7 @@
     <row r="18" spans="1:10" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="37"/>
       <c r="B18" s="42">
-        <f>ROW(B18) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C18" s="43"/>
@@ -1735,16 +1740,16 @@
         <v>1</v>
       </c>
       <c r="E18" s="66" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F18" s="66" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G18" s="66" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H18" s="66" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I18" s="44"/>
       <c r="J18" s="45"/>
@@ -1752,7 +1757,7 @@
     <row r="19" spans="1:10" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="46">
-        <f>ROW(B19) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C19" s="47"/>
@@ -1760,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="E19" s="67" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F19" s="67" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G19" s="67" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H19" s="67" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I19" s="47"/>
       <c r="J19" s="48"/>
@@ -1777,7 +1782,7 @@
     <row r="20" spans="1:10" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37"/>
       <c r="B20" s="42">
-        <f>ROW(B20) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C20" s="43"/>
@@ -1785,16 +1790,16 @@
         <v>1</v>
       </c>
       <c r="E20" s="66" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G20" s="66" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H20" s="66" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I20" s="44"/>
       <c r="J20" s="45"/>
@@ -1802,7 +1807,7 @@
     <row r="21" spans="1:10" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="46">
-        <f>ROW(B21) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C21" s="47"/>
@@ -1810,16 +1815,16 @@
         <v>1</v>
       </c>
       <c r="E21" s="67" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F21" s="67" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G21" s="67" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H21" s="67" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I21" s="47"/>
       <c r="J21" s="48"/>
@@ -1827,7 +1832,7 @@
     <row r="22" spans="1:10" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37"/>
       <c r="B22" s="42">
-        <f>ROW(B22) - ROW($B$9)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C22" s="43"/>
@@ -1835,16 +1840,16 @@
         <v>1</v>
       </c>
       <c r="E22" s="66" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F22" s="66" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G22" s="66" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H22" s="66" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I22" s="44"/>
       <c r="J22" s="45"/>
@@ -1963,7 +1968,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1995,7 +2000,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="70" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2035,7 +2040,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2043,7 +2048,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2051,7 +2056,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2059,7 +2064,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="70" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2067,7 +2072,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>